<commit_message>
finalizing work on map
</commit_message>
<xml_diff>
--- a/Original Plot Work/Womans Suffrage Timeline/data3.xlsx
+++ b/Original Plot Work/Womans Suffrage Timeline/data3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\R_Work\Slow_Reveal_Graphs\Original Plot Work\Womans Suffrage Timeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\R_work\Slow_Reveal_Graphs\Original Plot Work\Womans Suffrage Timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0194926-0694-45BE-8711-649D45BEA41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C121E6F1-ED81-4872-AD7D-89F5385A678A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{A2B69022-1D9E-493D-ABC5-004A2EBF399C}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{A2B69022-1D9E-493D-ABC5-004A2EBF399C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>